<commit_message>
created bpp trend pre-release branch
</commit_message>
<xml_diff>
--- a/data/BppTrend/BOE Equipment Index Factors and Percent Good Factors Sample.xlsx
+++ b/data/BppTrend/BOE Equipment Index Factors and Percent Good Factors Sample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yogsingh5\Downloads\sample data files\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sikbhamb\Project\APAS_Automation\qa_automation\data\BppTrend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" tabRatio="790" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Document Details" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Tabs</t>
   </si>
@@ -168,7 +168,10 @@
     <t>Harvesters - Average</t>
   </si>
   <si>
-    <t>sd</t>
+    <t>Junk_A</t>
+  </si>
+  <si>
+    <t>Junk_B</t>
   </si>
 </sst>
 </file>
@@ -251,7 +254,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -290,6 +293,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,13 +613,13 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.54296875" customWidth="1"/>
+    <col min="3" max="3" width="48.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="13">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -693,17 +699,17 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="12.453125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="13">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -711,23 +717,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="13">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
-      <c r="B2" s="8">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
       <c r="A3" s="8">
         <v>2018</v>
       </c>
-      <c r="B3" s="8">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="B3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="13">
       <c r="A4" s="6">
         <v>2017</v>
       </c>
@@ -737,7 +743,7 @@
       <c r="C4" s="5"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="13">
       <c r="A5" s="6">
         <v>2016</v>
       </c>
@@ -747,7 +753,7 @@
       <c r="C5" s="5"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" ht="13">
       <c r="A6" s="6">
         <v>2015</v>
       </c>
@@ -757,7 +763,7 @@
       <c r="C6" s="5"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="13">
       <c r="A7" s="6">
         <v>2014</v>
       </c>
@@ -767,7 +773,7 @@
       <c r="C7" s="5"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="13">
       <c r="A8" s="6">
         <v>2013</v>
       </c>
@@ -777,7 +783,7 @@
       <c r="C8" s="5"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" ht="13">
       <c r="A9" s="6">
         <v>2012</v>
       </c>
@@ -787,7 +793,7 @@
       <c r="C9" s="5"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" ht="13">
       <c r="A10" s="6">
         <v>2011</v>
       </c>
@@ -797,7 +803,7 @@
       <c r="C10" s="5"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="13">
       <c r="A11" s="6">
         <v>2010</v>
       </c>
@@ -807,7 +813,7 @@
       <c r="C11" s="5"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="13">
       <c r="A12" s="6">
         <v>2009</v>
       </c>
@@ -817,7 +823,7 @@
       <c r="C12" s="5"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="13">
       <c r="A13" s="6">
         <v>2008</v>
       </c>
@@ -827,7 +833,7 @@
       <c r="C13" s="5"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="13">
       <c r="A14" s="6">
         <v>2007</v>
       </c>
@@ -837,7 +843,7 @@
       <c r="C14" s="5"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="13">
       <c r="A15" s="6">
         <v>2006</v>
       </c>
@@ -847,7 +853,7 @@
       <c r="C15" s="5"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="13">
       <c r="A16" s="6">
         <v>2005</v>
       </c>
@@ -857,7 +863,7 @@
       <c r="C16" s="5"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="13">
       <c r="A17" s="6">
         <v>2004</v>
       </c>
@@ -867,7 +873,7 @@
       <c r="C17" s="5"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="13">
       <c r="A18" s="6">
         <v>2003</v>
       </c>
@@ -877,7 +883,7 @@
       <c r="C18" s="5"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="13">
       <c r="A19" s="6">
         <v>2002</v>
       </c>
@@ -887,7 +893,7 @@
       <c r="C19" s="5"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="13">
       <c r="A20" s="6">
         <v>2001</v>
       </c>
@@ -897,7 +903,7 @@
       <c r="C20" s="5"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="13">
       <c r="A21" s="6">
         <v>2000</v>
       </c>
@@ -907,7 +913,7 @@
       <c r="C21" s="5"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="13">
       <c r="A22" s="6">
         <v>1999</v>
       </c>
@@ -917,7 +923,7 @@
       <c r="C22" s="5"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="13">
       <c r="A23" s="6">
         <v>1998</v>
       </c>
@@ -927,7 +933,7 @@
       <c r="C23" s="5"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="13">
       <c r="A24" s="6">
         <v>1997</v>
       </c>
@@ -937,7 +943,7 @@
       <c r="C24" s="5"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="13">
       <c r="A25" s="6">
         <v>1996</v>
       </c>
@@ -947,7 +953,7 @@
       <c r="C25" s="5"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" ht="13">
       <c r="A26" s="6">
         <v>1995</v>
       </c>
@@ -957,7 +963,7 @@
       <c r="C26" s="5"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" ht="13">
       <c r="A27" s="6">
         <v>1994</v>
       </c>
@@ -967,7 +973,7 @@
       <c r="C27" s="5"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" ht="13">
       <c r="A28" s="6">
         <v>1993</v>
       </c>
@@ -977,7 +983,7 @@
       <c r="C28" s="5"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" ht="13">
       <c r="A29" s="6">
         <v>1992</v>
       </c>
@@ -987,7 +993,7 @@
       <c r="C29" s="5"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" ht="13">
       <c r="A30" s="6">
         <v>1991</v>
       </c>
@@ -997,7 +1003,7 @@
       <c r="C30" s="5"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" ht="13">
       <c r="A31" s="6">
         <v>1990</v>
       </c>
@@ -1007,7 +1013,7 @@
       <c r="C31" s="5"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" ht="13">
       <c r="A32" s="6">
         <v>1989</v>
       </c>
@@ -1017,7 +1023,7 @@
       <c r="C32" s="5"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="13">
       <c r="A33" s="6">
         <v>1988</v>
       </c>
@@ -1027,7 +1033,7 @@
       <c r="C33" s="5"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" ht="13">
       <c r="A34" s="6">
         <v>1987</v>
       </c>
@@ -1037,7 +1043,7 @@
       <c r="C34" s="5"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" ht="13">
       <c r="A35" s="6">
         <v>1986</v>
       </c>
@@ -1047,7 +1053,7 @@
       <c r="C35" s="5"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" ht="13">
       <c r="A36" s="6">
         <v>1985</v>
       </c>
@@ -1057,7 +1063,7 @@
       <c r="C36" s="5"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" ht="13">
       <c r="A37" s="6">
         <v>1984</v>
       </c>
@@ -1067,7 +1073,7 @@
       <c r="C37" s="5"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" ht="13">
       <c r="A38" s="6">
         <v>1983</v>
       </c>
@@ -1077,105 +1083,105 @@
       <c r="C38" s="5"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" ht="13">
       <c r="A39" s="6"/>
       <c r="B39" s="2"/>
       <c r="C39" s="5"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" ht="13">
       <c r="A40" s="6"/>
       <c r="B40" s="2"/>
       <c r="C40" s="5"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="13">
       <c r="A41" s="6"/>
       <c r="B41" s="2"/>
       <c r="C41" s="5"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" ht="13">
       <c r="A42" s="6"/>
       <c r="B42" s="2"/>
       <c r="C42" s="5"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" ht="13">
       <c r="A43" s="6"/>
       <c r="B43" s="2"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" ht="13">
       <c r="C44" s="5"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" ht="13">
       <c r="C45" s="5"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" ht="13">
       <c r="C46" s="5"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" ht="13">
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" ht="13">
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="3:3">
+    <row r="49" spans="3:3" ht="13">
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="3:3" ht="13">
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="3:3">
+    <row r="51" spans="3:3" ht="13">
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="3:3">
+    <row r="52" spans="3:3" ht="13">
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="3:3" ht="13">
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="3:3" ht="13">
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="3:3" ht="13">
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="3:3">
+    <row r="56" spans="3:3" ht="13">
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="3:3" ht="13">
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="3:3" ht="13">
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="3:3" ht="13">
       <c r="C59" s="5"/>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="3:3" ht="13">
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="3:3" ht="13">
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="3:3">
+    <row r="62" spans="3:3" ht="13">
       <c r="C62" s="5"/>
     </row>
-    <row r="63" spans="3:3">
+    <row r="63" spans="3:3" ht="13">
       <c r="C63" s="5"/>
     </row>
-    <row r="64" spans="3:3">
+    <row r="64" spans="3:3" ht="13">
       <c r="C64" s="5"/>
     </row>
-    <row r="65" spans="3:3">
+    <row r="65" spans="3:3" ht="13">
       <c r="C65" s="5"/>
     </row>
-    <row r="66" spans="3:3">
+    <row r="66" spans="3:3" ht="13">
       <c r="C66" s="5"/>
     </row>
-    <row r="67" spans="3:3">
+    <row r="67" spans="3:3" ht="13">
       <c r="C67" s="5"/>
     </row>
   </sheetData>
@@ -1191,18 +1197,18 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="13">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -1211,21 +1217,21 @@
       </c>
       <c r="C1" s="13"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="13">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
-      <c r="B2" s="8">
-        <v>105</v>
+      <c r="B2" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="13"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="13">
       <c r="A3" s="8">
         <v>2018</v>
       </c>
-      <c r="B3" s="8">
-        <v>104</v>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="13"/>
     </row>
@@ -1505,18 +1511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="13">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -1524,20 +1528,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
-      <c r="B2" s="8">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13">
       <c r="A3" s="8">
         <v>2018</v>
       </c>
-      <c r="B3" s="8">
-        <v>103</v>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1696,8 +1700,8 @@
       <c r="A23" s="6">
         <v>1998</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>43</v>
+      <c r="B23" s="2">
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1868,17 +1872,17 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.1796875" style="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="13">
       <c r="A1" s="8" t="s">
         <v>18</v>
       </c>
@@ -1886,20 +1890,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" s="8">
         <v>2019</v>
       </c>
-      <c r="B2" s="8">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13">
       <c r="A3" s="8">
         <v>2018</v>
       </c>
-      <c r="B3" s="8">
-        <v>105</v>
+      <c r="B3" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2238,31 +2242,32 @@
   <dimension ref="A1:AG42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="2.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="2.81640625" style="1" customWidth="1"/>
     <col min="16" max="19" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="1"/>
-    <col min="27" max="27" width="35.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="12.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.1796875" style="1"/>
+    <col min="27" max="27" width="35.26953125" style="1" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="12.81640625" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="31" max="32" width="11.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="12.453125" style="1" hidden="1" customWidth="1"/>
+    <col min="31" max="32" width="11.453125" style="1" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="16" style="1" hidden="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="34" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" ht="13">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -2339,15 +2344,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" ht="13">
       <c r="A2">
         <v>2019</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>39</v>
+      <c r="C2" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D2" s="2">
         <v>55</v>
@@ -2416,15 +2421,15 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" ht="13">
       <c r="A3">
         <v>2018</v>
       </c>
       <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>37</v>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="D3" s="2">
         <v>52</v>
@@ -2493,7 +2498,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" ht="13">
       <c r="A4" s="7">
         <v>2017</v>
       </c>
@@ -2585,7 +2590,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" ht="13">
       <c r="A5" s="6">
         <v>2016</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" ht="13">
       <c r="A6" s="6">
         <v>2015</v>
       </c>
@@ -2759,7 +2764,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" ht="13">
       <c r="A7" s="6">
         <v>2014</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>38.479999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" ht="13">
       <c r="A8" s="6">
         <v>2013</v>
       </c>
@@ -2951,7 +2956,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" ht="13">
       <c r="A9" s="6">
         <v>2012</v>
       </c>
@@ -3201,7 +3206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" ht="13">
       <c r="A12" s="6">
         <v>2009</v>
       </c>
@@ -3279,7 +3284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" ht="13">
       <c r="A13" s="6">
         <v>2008</v>
       </c>
@@ -3352,7 +3357,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" ht="13">
       <c r="A14" s="6">
         <v>2007</v>
       </c>
@@ -3423,7 +3428,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" ht="13">
       <c r="A15" s="6">
         <v>2006</v>
       </c>
@@ -3491,7 +3496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" ht="13">
       <c r="A16" s="6">
         <v>2005</v>
       </c>
@@ -3554,7 +3559,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" ht="13">
       <c r="A17" s="6">
         <v>2004</v>
       </c>
@@ -3617,7 +3622,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="14.25">
+    <row r="18" spans="1:33" ht="14">
       <c r="A18" s="6">
         <v>2003</v>
       </c>
@@ -3688,7 +3693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" ht="13">
       <c r="A19" s="6">
         <v>2002</v>
       </c>
@@ -3753,7 +3758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" ht="13">
       <c r="A20" s="6">
         <v>2001</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" ht="13">
       <c r="A21" s="6">
         <v>2000</v>
       </c>
@@ -3869,7 +3874,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" ht="13">
       <c r="A22" s="6">
         <v>1999</v>
       </c>
@@ -3934,7 +3939,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" ht="13">
       <c r="A23" s="6">
         <v>1998</v>
       </c>
@@ -3999,7 +4004,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" ht="13">
       <c r="A24" s="6">
         <v>1997</v>
       </c>
@@ -4052,7 +4057,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" ht="13">
       <c r="A25" s="6">
         <v>1996</v>
       </c>
@@ -4105,7 +4110,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" ht="13">
       <c r="A26" s="6">
         <v>1995</v>
       </c>
@@ -4158,7 +4163,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" ht="13">
       <c r="A27" s="6">
         <v>1994</v>
       </c>
@@ -4230,7 +4235,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" ht="13">
       <c r="A28" s="6">
         <v>1993</v>
       </c>
@@ -4303,7 +4308,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" ht="13">
       <c r="A29" s="6">
         <v>1992</v>
       </c>
@@ -4357,7 +4362,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" ht="13">
       <c r="A30" s="6">
         <v>1991</v>
       </c>
@@ -4411,7 +4416,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" ht="13">
       <c r="A31" s="6">
         <v>1990</v>
       </c>
@@ -4463,7 +4468,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" ht="13">
       <c r="A32" s="6">
         <v>1989</v>
       </c>
@@ -4515,7 +4520,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" ht="13">
       <c r="A33" s="6">
         <v>1988</v>
       </c>
@@ -4562,7 +4567,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" ht="13">
       <c r="A34" s="6">
         <v>1987</v>
       </c>
@@ -4607,7 +4612,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" ht="13">
       <c r="A35" s="6">
         <v>1986</v>
       </c>
@@ -4652,7 +4657,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" ht="13">
       <c r="A36" s="6">
         <v>1985</v>
       </c>
@@ -4697,7 +4702,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" ht="13">
       <c r="A37" s="6">
         <v>1984</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" ht="13">
       <c r="A38" s="6">
         <v>1983</v>
       </c>
@@ -4783,7 +4788,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" ht="13">
       <c r="A39" s="6">
         <v>1982</v>
       </c>
@@ -4826,7 +4831,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" ht="13">
       <c r="A40" s="6">
         <v>1981</v>
       </c>
@@ -4869,7 +4874,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" ht="13">
       <c r="A41" s="6">
         <v>1980</v>
       </c>
@@ -4928,13 +4933,13 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4954,7 +4959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="13">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -4967,11 +4972,11 @@
       <c r="D2">
         <v>81</v>
       </c>
-      <c r="E2">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -4984,8 +4989,8 @@
       <c r="D3">
         <v>81</v>
       </c>
-      <c r="E3">
-        <v>74</v>
+      <c r="E3" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5337,21 +5342,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5383,7 +5388,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="13">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -5405,14 +5410,14 @@
       <c r="G2">
         <v>45</v>
       </c>
-      <c r="H2">
-        <v>67</v>
+      <c r="H2" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="13">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -5434,8 +5439,8 @@
       <c r="G3">
         <v>67</v>
       </c>
-      <c r="H3">
-        <v>78</v>
+      <c r="H3" s="16" t="s">
+        <v>44</v>
       </c>
       <c r="I3">
         <v>2</v>

</xml_diff>